<commit_message>
added excel controller, needs refactoring
</commit_message>
<xml_diff>
--- a/templates/leave-form-template2.xlsx
+++ b/templates/leave-form-template2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Management System\backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7253A5-0467-41D0-80F6-276444D04480}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B823D42E-BC54-4367-8677-3885942EAA8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1113,8 +1113,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1122,22 +1150,22 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1212,18 +1240,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1248,51 +1264,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2854,8 +2854,8 @@
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>171879</xdr:colOff>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
@@ -2921,8 +2921,8 @@
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>171879</xdr:colOff>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -3323,8 +3323,8 @@
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>171879</xdr:colOff>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>29</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -3390,8 +3390,8 @@
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>171879</xdr:colOff>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
@@ -8715,8 +8715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="133" zoomScaleNormal="100" zoomScaleSheetLayoutView="126" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M2"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="133" zoomScaleNormal="100" zoomScaleSheetLayoutView="126" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8737,54 +8737,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
       <c r="J1" s="53"/>
       <c r="K1" s="53"/>
       <c r="L1" s="55"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
+      <c r="A2" s="136"/>
+      <c r="B2" s="136"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="136"/>
+      <c r="M2" s="136"/>
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84"/>
+      <c r="B3" s="137"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="137"/>
+      <c r="M3" s="137"/>
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8816,20 +8816,20 @@
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="138" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="139"/>
       <c r="E5" s="54"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
+      <c r="F5" s="140"/>
+      <c r="G5" s="140"/>
+      <c r="H5" s="140"/>
       <c r="I5" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
+      <c r="J5" s="140"/>
+      <c r="K5" s="140"/>
       <c r="L5" s="66"/>
       <c r="M5" s="65"/>
     </row>
@@ -8837,24 +8837,24 @@
       <c r="A6" s="62">
         <v>3</v>
       </c>
-      <c r="B6" s="128" t="s">
+      <c r="B6" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="128"/>
+      <c r="C6" s="90"/>
       <c r="D6" s="67"/>
       <c r="E6" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
       <c r="I6" s="5"/>
       <c r="J6" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="K6" s="142"/>
-      <c r="L6" s="142"/>
-      <c r="M6" s="143"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="100"/>
+      <c r="M6" s="101"/>
     </row>
     <row r="7" spans="1:15" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
@@ -8873,20 +8873,20 @@
     </row>
     <row r="8" spans="1:15" s="16" customFormat="1" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
-      <c r="B8" s="112" t="s">
+      <c r="B8" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="112"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="112"/>
-      <c r="I8" s="112"/>
-      <c r="J8" s="112"/>
-      <c r="K8" s="112"/>
-      <c r="L8" s="112"/>
-      <c r="M8" s="113"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="96"/>
+      <c r="J8" s="96"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
+      <c r="M8" s="97"/>
     </row>
     <row r="9" spans="1:15" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
@@ -8934,14 +8934,14 @@
       <c r="E11" s="21"/>
       <c r="F11" s="22"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="80" t="s">
+      <c r="H11" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="80"/>
-      <c r="J11" s="80"/>
-      <c r="K11" s="80"/>
-      <c r="L11" s="80"/>
-      <c r="M11" s="81"/>
+      <c r="I11" s="94"/>
+      <c r="J11" s="94"/>
+      <c r="K11" s="94"/>
+      <c r="L11" s="94"/>
+      <c r="M11" s="95"/>
     </row>
     <row r="12" spans="1:15" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
@@ -9040,14 +9040,14 @@
       <c r="E17" s="21"/>
       <c r="F17" s="22"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="80" t="s">
+      <c r="H17" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="80"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="80"/>
-      <c r="L17" s="80"/>
-      <c r="M17" s="81"/>
+      <c r="I17" s="94"/>
+      <c r="J17" s="94"/>
+      <c r="K17" s="94"/>
+      <c r="L17" s="94"/>
+      <c r="M17" s="95"/>
     </row>
     <row r="18" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
@@ -9178,14 +9178,14 @@
       <c r="E25" s="21"/>
       <c r="F25" s="22"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="80" t="s">
+      <c r="H25" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="I25" s="80"/>
-      <c r="J25" s="80"/>
-      <c r="K25" s="80"/>
-      <c r="L25" s="80"/>
-      <c r="M25" s="81"/>
+      <c r="I25" s="94"/>
+      <c r="J25" s="94"/>
+      <c r="K25" s="94"/>
+      <c r="L25" s="94"/>
+      <c r="M25" s="95"/>
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9267,21 +9267,21 @@
     <row r="31" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="132" t="s">
+      <c r="C31" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="132"/>
-      <c r="E31" s="132"/>
-      <c r="F31" s="133"/>
+      <c r="D31" s="98"/>
+      <c r="E31" s="98"/>
+      <c r="F31" s="99"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="80" t="s">
+      <c r="H31" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="I31" s="80"/>
-      <c r="J31" s="80"/>
-      <c r="K31" s="80"/>
-      <c r="L31" s="80"/>
-      <c r="M31" s="81"/>
+      <c r="I31" s="94"/>
+      <c r="J31" s="94"/>
+      <c r="K31" s="94"/>
+      <c r="L31" s="94"/>
+      <c r="M31" s="95"/>
       <c r="N31" s="2"/>
     </row>
     <row r="32" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9311,13 +9311,13 @@
       <c r="F33" s="22"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
-      <c r="I33" s="114" t="s">
+      <c r="I33" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="J33" s="114"/>
-      <c r="K33" s="114"/>
-      <c r="L33" s="114"/>
-      <c r="M33" s="115"/>
+      <c r="J33" s="88"/>
+      <c r="K33" s="88"/>
+      <c r="L33" s="88"/>
+      <c r="M33" s="89"/>
       <c r="N33" s="2"/>
     </row>
     <row r="34" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9346,13 +9346,13 @@
       <c r="F35" s="14"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
-      <c r="I35" s="114" t="s">
+      <c r="I35" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="J35" s="114"/>
-      <c r="K35" s="114"/>
-      <c r="L35" s="114"/>
-      <c r="M35" s="115"/>
+      <c r="J35" s="88"/>
+      <c r="K35" s="88"/>
+      <c r="L35" s="88"/>
+      <c r="M35" s="89"/>
     </row>
     <row r="36" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
@@ -9373,14 +9373,14 @@
       <c r="E37" s="2"/>
       <c r="F37" s="14"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="126" t="s">
+      <c r="H37" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="I37" s="126"/>
-      <c r="J37" s="126"/>
-      <c r="K37" s="126"/>
-      <c r="L37" s="126"/>
-      <c r="M37" s="127"/>
+      <c r="I37" s="86"/>
+      <c r="J37" s="86"/>
+      <c r="K37" s="86"/>
+      <c r="L37" s="86"/>
+      <c r="M37" s="87"/>
     </row>
     <row r="38" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
@@ -9410,13 +9410,13 @@
       <c r="H39" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="I39" s="114" t="s">
+      <c r="I39" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="J39" s="114"/>
-      <c r="K39" s="114"/>
-      <c r="L39" s="114"/>
-      <c r="M39" s="115"/>
+      <c r="J39" s="88"/>
+      <c r="K39" s="88"/>
+      <c r="L39" s="88"/>
+      <c r="M39" s="89"/>
     </row>
     <row r="40" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
@@ -9446,13 +9446,13 @@
       <c r="H41" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="I41" s="114" t="s">
+      <c r="I41" s="88" t="s">
         <v>39</v>
       </c>
-      <c r="J41" s="114"/>
-      <c r="K41" s="114"/>
-      <c r="L41" s="114"/>
-      <c r="M41" s="115"/>
+      <c r="J41" s="88"/>
+      <c r="K41" s="88"/>
+      <c r="L41" s="88"/>
+      <c r="M41" s="89"/>
     </row>
     <row r="42" spans="1:16" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
@@ -9483,8 +9483,8 @@
       </c>
       <c r="H43" s="30"/>
       <c r="M43" s="26"/>
-      <c r="O43" s="88"/>
-      <c r="P43" s="89"/>
+      <c r="O43" s="102"/>
+      <c r="P43" s="103"/>
     </row>
     <row r="44" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="29"/>
@@ -9499,20 +9499,20 @@
     </row>
     <row r="45" spans="1:16" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
-      <c r="B45" s="131"/>
-      <c r="C45" s="131"/>
-      <c r="D45" s="131"/>
-      <c r="E45" s="131"/>
+      <c r="B45" s="93"/>
+      <c r="C45" s="93"/>
+      <c r="D45" s="93"/>
+      <c r="E45" s="93"/>
       <c r="F45" s="14"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
-      <c r="I45" s="129" t="s">
+      <c r="I45" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="J45" s="129"/>
-      <c r="K45" s="129"/>
-      <c r="L45" s="129"/>
-      <c r="M45" s="130"/>
+      <c r="J45" s="91"/>
+      <c r="K45" s="91"/>
+      <c r="L45" s="91"/>
+      <c r="M45" s="92"/>
     </row>
     <row r="46" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
@@ -9540,19 +9540,19 @@
       <c r="F47" s="14"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
-      <c r="I47" s="114" t="s">
+      <c r="I47" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="J47" s="114"/>
-      <c r="K47" s="114"/>
-      <c r="L47" s="114"/>
-      <c r="M47" s="115"/>
+      <c r="J47" s="88"/>
+      <c r="K47" s="88"/>
+      <c r="L47" s="88"/>
+      <c r="M47" s="89"/>
     </row>
     <row r="48" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="31"/>
-      <c r="C48" s="90"/>
-      <c r="D48" s="91"/>
+      <c r="C48" s="104"/>
+      <c r="D48" s="105"/>
       <c r="E48" s="2"/>
       <c r="F48" s="14"/>
       <c r="G48" s="2"/>
@@ -9580,58 +9580,58 @@
     </row>
     <row r="50" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11"/>
-      <c r="B50" s="119" t="s">
+      <c r="B50" s="129" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="120"/>
-      <c r="D50" s="120"/>
-      <c r="E50" s="120"/>
+      <c r="C50" s="130"/>
+      <c r="D50" s="130"/>
+      <c r="E50" s="130"/>
       <c r="F50" s="14"/>
-      <c r="G50" s="116" t="s">
+      <c r="G50" s="126" t="s">
         <v>83</v>
       </c>
-      <c r="H50" s="117"/>
-      <c r="I50" s="117"/>
-      <c r="J50" s="117"/>
-      <c r="K50" s="117"/>
-      <c r="L50" s="117"/>
-      <c r="M50" s="118"/>
+      <c r="H50" s="127"/>
+      <c r="I50" s="127"/>
+      <c r="J50" s="127"/>
+      <c r="K50" s="127"/>
+      <c r="L50" s="127"/>
+      <c r="M50" s="128"/>
     </row>
     <row r="51" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="121" t="s">
+      <c r="A51" s="131" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="122"/>
-      <c r="C51" s="122"/>
-      <c r="D51" s="122"/>
-      <c r="E51" s="122"/>
-      <c r="F51" s="123"/>
-      <c r="G51" s="92" t="s">
+      <c r="B51" s="132"/>
+      <c r="C51" s="132"/>
+      <c r="D51" s="132"/>
+      <c r="E51" s="132"/>
+      <c r="F51" s="133"/>
+      <c r="G51" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="H51" s="93"/>
-      <c r="I51" s="93"/>
-      <c r="J51" s="93"/>
-      <c r="K51" s="93"/>
-      <c r="L51" s="93"/>
-      <c r="M51" s="94"/>
+      <c r="H51" s="107"/>
+      <c r="I51" s="107"/>
+      <c r="J51" s="107"/>
+      <c r="K51" s="107"/>
+      <c r="L51" s="107"/>
+      <c r="M51" s="108"/>
     </row>
     <row r="52" spans="1:13" s="16" customFormat="1" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
-      <c r="B52" s="112" t="s">
+      <c r="B52" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="112"/>
-      <c r="D52" s="112"/>
-      <c r="E52" s="112"/>
-      <c r="F52" s="112"/>
-      <c r="G52" s="112"/>
-      <c r="H52" s="112"/>
-      <c r="I52" s="112"/>
-      <c r="J52" s="112"/>
-      <c r="K52" s="112"/>
-      <c r="L52" s="112"/>
-      <c r="M52" s="113"/>
+      <c r="C52" s="96"/>
+      <c r="D52" s="96"/>
+      <c r="E52" s="96"/>
+      <c r="F52" s="96"/>
+      <c r="G52" s="96"/>
+      <c r="H52" s="96"/>
+      <c r="I52" s="96"/>
+      <c r="J52" s="96"/>
+      <c r="K52" s="96"/>
+      <c r="L52" s="96"/>
+      <c r="M52" s="97"/>
     </row>
     <row r="53" spans="1:13" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
@@ -9677,13 +9677,13 @@
       <c r="F55" s="14"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
-      <c r="I55" s="124" t="s">
+      <c r="I55" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="J55" s="124"/>
-      <c r="K55" s="124"/>
-      <c r="L55" s="124"/>
-      <c r="M55" s="125"/>
+      <c r="J55" s="84"/>
+      <c r="K55" s="84"/>
+      <c r="L55" s="84"/>
+      <c r="M55" s="85"/>
     </row>
     <row r="56" spans="1:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11"/>
@@ -9732,13 +9732,13 @@
       <c r="F58" s="14"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
-      <c r="I58" s="124" t="s">
+      <c r="I58" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="J58" s="124"/>
-      <c r="K58" s="124"/>
-      <c r="L58" s="124"/>
-      <c r="M58" s="125"/>
+      <c r="J58" s="84"/>
+      <c r="K58" s="84"/>
+      <c r="L58" s="84"/>
+      <c r="M58" s="85"/>
     </row>
     <row r="59" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11"/>
@@ -9751,13 +9751,13 @@
       <c r="F59" s="14"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
-      <c r="I59" s="124" t="s">
+      <c r="I59" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="J59" s="124"/>
-      <c r="K59" s="124"/>
-      <c r="L59" s="124"/>
-      <c r="M59" s="125"/>
+      <c r="J59" s="84"/>
+      <c r="K59" s="84"/>
+      <c r="L59" s="84"/>
+      <c r="M59" s="85"/>
     </row>
     <row r="60" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="11"/>
@@ -9770,44 +9770,44 @@
       <c r="F60" s="14"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
-      <c r="I60" s="124" t="s">
+      <c r="I60" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="J60" s="124"/>
-      <c r="K60" s="124"/>
-      <c r="L60" s="124"/>
-      <c r="M60" s="125"/>
+      <c r="J60" s="84"/>
+      <c r="K60" s="84"/>
+      <c r="L60" s="84"/>
+      <c r="M60" s="85"/>
     </row>
     <row r="61" spans="1:13" s="45" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="44"/>
-      <c r="G61" s="134" t="s">
+      <c r="G61" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="H61" s="135"/>
-      <c r="I61" s="135"/>
-      <c r="J61" s="135"/>
-      <c r="K61" s="135"/>
-      <c r="L61" s="135"/>
-      <c r="M61" s="136"/>
+      <c r="H61" s="80"/>
+      <c r="I61" s="80"/>
+      <c r="J61" s="80"/>
+      <c r="K61" s="80"/>
+      <c r="L61" s="80"/>
+      <c r="M61" s="81"/>
     </row>
     <row r="62" spans="1:13" s="49" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="47"/>
       <c r="B62" s="37"/>
-      <c r="C62" s="96" t="s">
+      <c r="C62" s="110" t="s">
         <v>62</v>
       </c>
-      <c r="D62" s="96"/>
-      <c r="E62" s="96"/>
+      <c r="D62" s="110"/>
+      <c r="E62" s="110"/>
       <c r="F62" s="48"/>
-      <c r="G62" s="97" t="s">
+      <c r="G62" s="111" t="s">
         <v>73</v>
       </c>
-      <c r="H62" s="98"/>
-      <c r="I62" s="93"/>
-      <c r="J62" s="93"/>
-      <c r="K62" s="93"/>
-      <c r="L62" s="93"/>
-      <c r="M62" s="99"/>
+      <c r="H62" s="112"/>
+      <c r="I62" s="107"/>
+      <c r="J62" s="107"/>
+      <c r="K62" s="107"/>
+      <c r="L62" s="107"/>
+      <c r="M62" s="113"/>
     </row>
     <row r="63" spans="1:13" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
@@ -9837,14 +9837,14 @@
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="137" t="s">
+      <c r="H64" s="82" t="s">
         <v>66</v>
       </c>
-      <c r="I64" s="137"/>
-      <c r="J64" s="137"/>
-      <c r="K64" s="137"/>
-      <c r="L64" s="137"/>
-      <c r="M64" s="138"/>
+      <c r="I64" s="82"/>
+      <c r="J64" s="82"/>
+      <c r="K64" s="82"/>
+      <c r="L64" s="82"/>
+      <c r="M64" s="83"/>
     </row>
     <row r="65" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="11"/>
@@ -9855,14 +9855,14 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="H65" s="124" t="s">
+      <c r="H65" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="I65" s="124"/>
-      <c r="J65" s="124"/>
-      <c r="K65" s="124"/>
-      <c r="L65" s="124"/>
-      <c r="M65" s="125"/>
+      <c r="I65" s="84"/>
+      <c r="J65" s="84"/>
+      <c r="K65" s="84"/>
+      <c r="L65" s="84"/>
+      <c r="M65" s="85"/>
     </row>
     <row r="66" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="11"/>
@@ -9873,14 +9873,14 @@
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-      <c r="H66" s="124" t="s">
+      <c r="H66" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="I66" s="124"/>
-      <c r="J66" s="124"/>
-      <c r="K66" s="124"/>
-      <c r="L66" s="124"/>
-      <c r="M66" s="125"/>
+      <c r="I66" s="84"/>
+      <c r="J66" s="84"/>
+      <c r="K66" s="84"/>
+      <c r="L66" s="84"/>
+      <c r="M66" s="85"/>
     </row>
     <row r="67" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="11"/>
@@ -9897,110 +9897,96 @@
       <c r="M67" s="14"/>
     </row>
     <row r="68" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="100" t="s">
+      <c r="A68" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="101"/>
-      <c r="C68" s="101"/>
-      <c r="D68" s="101"/>
-      <c r="E68" s="101"/>
-      <c r="F68" s="101"/>
-      <c r="G68" s="101"/>
-      <c r="H68" s="101"/>
-      <c r="I68" s="101"/>
-      <c r="J68" s="101"/>
-      <c r="K68" s="101"/>
-      <c r="L68" s="101"/>
-      <c r="M68" s="102"/>
+      <c r="B68" s="115"/>
+      <c r="C68" s="115"/>
+      <c r="D68" s="115"/>
+      <c r="E68" s="115"/>
+      <c r="F68" s="115"/>
+      <c r="G68" s="115"/>
+      <c r="H68" s="115"/>
+      <c r="I68" s="115"/>
+      <c r="J68" s="115"/>
+      <c r="K68" s="115"/>
+      <c r="L68" s="115"/>
+      <c r="M68" s="116"/>
     </row>
     <row r="69" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="103" t="s">
+      <c r="A69" s="117" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="104"/>
-      <c r="C69" s="104"/>
-      <c r="D69" s="104"/>
-      <c r="E69" s="104"/>
-      <c r="F69" s="104"/>
-      <c r="G69" s="104"/>
-      <c r="H69" s="104"/>
-      <c r="I69" s="104"/>
-      <c r="J69" s="104"/>
-      <c r="K69" s="104"/>
-      <c r="L69" s="104"/>
-      <c r="M69" s="105"/>
+      <c r="B69" s="118"/>
+      <c r="C69" s="118"/>
+      <c r="D69" s="118"/>
+      <c r="E69" s="118"/>
+      <c r="F69" s="118"/>
+      <c r="G69" s="118"/>
+      <c r="H69" s="118"/>
+      <c r="I69" s="118"/>
+      <c r="J69" s="118"/>
+      <c r="K69" s="118"/>
+      <c r="L69" s="118"/>
+      <c r="M69" s="119"/>
     </row>
     <row r="70" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="106" t="s">
+      <c r="A70" s="120" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="107"/>
-      <c r="C70" s="107"/>
-      <c r="D70" s="107"/>
-      <c r="E70" s="107"/>
-      <c r="F70" s="107"/>
-      <c r="G70" s="107"/>
-      <c r="H70" s="107"/>
-      <c r="I70" s="107"/>
-      <c r="J70" s="107"/>
-      <c r="K70" s="107"/>
-      <c r="L70" s="107"/>
-      <c r="M70" s="108"/>
+      <c r="B70" s="121"/>
+      <c r="C70" s="121"/>
+      <c r="D70" s="121"/>
+      <c r="E70" s="121"/>
+      <c r="F70" s="121"/>
+      <c r="G70" s="121"/>
+      <c r="H70" s="121"/>
+      <c r="I70" s="121"/>
+      <c r="J70" s="121"/>
+      <c r="K70" s="121"/>
+      <c r="L70" s="121"/>
+      <c r="M70" s="122"/>
     </row>
     <row r="71" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="109" t="s">
+      <c r="A71" s="123" t="s">
         <v>72</v>
       </c>
-      <c r="B71" s="110"/>
-      <c r="C71" s="110"/>
-      <c r="D71" s="110"/>
-      <c r="E71" s="110"/>
-      <c r="F71" s="110"/>
-      <c r="G71" s="110"/>
-      <c r="H71" s="110"/>
-      <c r="I71" s="110"/>
-      <c r="J71" s="110"/>
-      <c r="K71" s="110"/>
-      <c r="L71" s="110"/>
-      <c r="M71" s="111"/>
+      <c r="B71" s="124"/>
+      <c r="C71" s="124"/>
+      <c r="D71" s="124"/>
+      <c r="E71" s="124"/>
+      <c r="F71" s="124"/>
+      <c r="G71" s="124"/>
+      <c r="H71" s="124"/>
+      <c r="I71" s="124"/>
+      <c r="J71" s="124"/>
+      <c r="K71" s="124"/>
+      <c r="L71" s="124"/>
+      <c r="M71" s="125"/>
     </row>
     <row r="72" spans="1:13" s="52" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="95"/>
-      <c r="B72" s="95"/>
-      <c r="C72" s="95"/>
-      <c r="D72" s="95"/>
-      <c r="E72" s="95"/>
-      <c r="F72" s="95"/>
-      <c r="G72" s="95"/>
-      <c r="H72" s="95"/>
-      <c r="I72" s="95"/>
-      <c r="J72" s="95"/>
-      <c r="K72" s="95"/>
-      <c r="L72" s="95"/>
-      <c r="M72" s="95"/>
+      <c r="A72" s="109"/>
+      <c r="B72" s="109"/>
+      <c r="C72" s="109"/>
+      <c r="D72" s="109"/>
+      <c r="E72" s="109"/>
+      <c r="F72" s="109"/>
+      <c r="G72" s="109"/>
+      <c r="H72" s="109"/>
+      <c r="I72" s="109"/>
+      <c r="J72" s="109"/>
+      <c r="K72" s="109"/>
+      <c r="L72" s="109"/>
+      <c r="M72" s="109"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="G61:M61"/>
-    <mergeCell ref="H64:M64"/>
-    <mergeCell ref="H65:M65"/>
-    <mergeCell ref="H66:M66"/>
-    <mergeCell ref="I58:M58"/>
-    <mergeCell ref="I59:M59"/>
-    <mergeCell ref="I60:M60"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="I41:M41"/>
-    <mergeCell ref="I39:M39"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="I45:M45"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="I35:M35"/>
-    <mergeCell ref="I33:M33"/>
-    <mergeCell ref="B8:M8"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="J5:K5"/>
     <mergeCell ref="O43:P43"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="G51:M51"/>
@@ -10017,15 +10003,29 @@
     <mergeCell ref="B50:E50"/>
     <mergeCell ref="A51:F51"/>
     <mergeCell ref="I55:M55"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="I41:M41"/>
+    <mergeCell ref="I39:M39"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="I45:M45"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="I35:M35"/>
+    <mergeCell ref="I33:M33"/>
+    <mergeCell ref="B8:M8"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="K6:M6"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="H11:M11"/>
     <mergeCell ref="H17:M17"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="G61:M61"/>
+    <mergeCell ref="H64:M64"/>
+    <mergeCell ref="H65:M65"/>
+    <mergeCell ref="H66:M66"/>
+    <mergeCell ref="I58:M58"/>
+    <mergeCell ref="I59:M59"/>
+    <mergeCell ref="I60:M60"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10612,42 +10612,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
+      <c r="A2" s="136"/>
+      <c r="B2" s="136"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
+      <c r="B3" s="137"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -10669,14 +10669,14 @@
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="139"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="140"/>
+      <c r="B5" s="142"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="139"/>
+      <c r="F5" s="139"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="143"/>
     </row>
     <row r="6" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
@@ -10705,16 +10705,16 @@
     </row>
     <row r="8" spans="1:11" s="16" customFormat="1" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
-      <c r="B8" s="112" t="s">
+      <c r="B8" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="112"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="112"/>
-      <c r="I8" s="113"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="97"/>
     </row>
     <row r="9" spans="1:11" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
@@ -11007,12 +11007,12 @@
     <row r="31" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="132" t="s">
+      <c r="C31" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="132"/>
-      <c r="E31" s="132"/>
-      <c r="F31" s="133"/>
+      <c r="D31" s="98"/>
+      <c r="E31" s="98"/>
+      <c r="F31" s="99"/>
       <c r="G31" s="2"/>
       <c r="H31" s="23" t="s">
         <v>30</v>
@@ -11173,8 +11173,8 @@
         <v>41</v>
       </c>
       <c r="I43" s="26"/>
-      <c r="K43" s="88"/>
-      <c r="L43" s="89"/>
+      <c r="K43" s="102"/>
+      <c r="L43" s="103"/>
     </row>
     <row r="44" spans="1:12" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="29"/>
@@ -11230,8 +11230,8 @@
     <row r="48" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
       <c r="B48" s="31"/>
-      <c r="C48" s="88"/>
-      <c r="D48" s="89"/>
+      <c r="C48" s="102"/>
+      <c r="D48" s="103"/>
       <c r="E48" s="2"/>
       <c r="F48" s="14"/>
       <c r="G48" s="2"/>
@@ -11269,30 +11269,30 @@
         <v>47</v>
       </c>
       <c r="B51" s="2"/>
-      <c r="C51" s="98" t="s">
+      <c r="C51" s="112" t="s">
         <v>73</v>
       </c>
-      <c r="D51" s="93"/>
+      <c r="D51" s="107"/>
       <c r="E51" s="37"/>
       <c r="F51" s="14"/>
       <c r="G51" s="141" t="s">
         <v>48</v>
       </c>
-      <c r="H51" s="93"/>
-      <c r="I51" s="94"/>
+      <c r="H51" s="107"/>
+      <c r="I51" s="108"/>
     </row>
     <row r="52" spans="1:9" s="16" customFormat="1" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
-      <c r="B52" s="112" t="s">
+      <c r="B52" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="112"/>
-      <c r="D52" s="112"/>
-      <c r="E52" s="112"/>
-      <c r="F52" s="112"/>
-      <c r="G52" s="112"/>
-      <c r="H52" s="112"/>
-      <c r="I52" s="113"/>
+      <c r="C52" s="96"/>
+      <c r="D52" s="96"/>
+      <c r="E52" s="96"/>
+      <c r="F52" s="96"/>
+      <c r="G52" s="96"/>
+      <c r="H52" s="96"/>
+      <c r="I52" s="97"/>
     </row>
     <row r="53" spans="1:9" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
@@ -11417,17 +11417,17 @@
     <row r="62" spans="1:9" s="49" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="47"/>
       <c r="B62" s="37"/>
-      <c r="C62" s="96" t="s">
+      <c r="C62" s="110" t="s">
         <v>62</v>
       </c>
-      <c r="D62" s="96"/>
-      <c r="E62" s="96"/>
+      <c r="D62" s="110"/>
+      <c r="E62" s="110"/>
       <c r="F62" s="48"/>
-      <c r="G62" s="97" t="s">
+      <c r="G62" s="111" t="s">
         <v>73</v>
       </c>
-      <c r="H62" s="93"/>
-      <c r="I62" s="99"/>
+      <c r="H62" s="107"/>
+      <c r="I62" s="113"/>
     </row>
     <row r="63" spans="1:9" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
@@ -11497,70 +11497,77 @@
       <c r="I67" s="14"/>
     </row>
     <row r="68" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="100" t="s">
+      <c r="A68" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="101"/>
-      <c r="C68" s="101"/>
-      <c r="D68" s="101"/>
-      <c r="E68" s="101"/>
-      <c r="F68" s="101"/>
-      <c r="G68" s="101"/>
-      <c r="H68" s="101"/>
-      <c r="I68" s="102"/>
+      <c r="B68" s="115"/>
+      <c r="C68" s="115"/>
+      <c r="D68" s="115"/>
+      <c r="E68" s="115"/>
+      <c r="F68" s="115"/>
+      <c r="G68" s="115"/>
+      <c r="H68" s="115"/>
+      <c r="I68" s="116"/>
     </row>
     <row r="69" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="103" t="s">
+      <c r="A69" s="117" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="104"/>
-      <c r="C69" s="104"/>
-      <c r="D69" s="104"/>
-      <c r="E69" s="104"/>
-      <c r="F69" s="104"/>
-      <c r="G69" s="104"/>
-      <c r="H69" s="104"/>
-      <c r="I69" s="105"/>
+      <c r="B69" s="118"/>
+      <c r="C69" s="118"/>
+      <c r="D69" s="118"/>
+      <c r="E69" s="118"/>
+      <c r="F69" s="118"/>
+      <c r="G69" s="118"/>
+      <c r="H69" s="118"/>
+      <c r="I69" s="119"/>
     </row>
     <row r="70" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="106" t="s">
+      <c r="A70" s="120" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="107"/>
-      <c r="C70" s="107"/>
-      <c r="D70" s="107"/>
-      <c r="E70" s="107"/>
-      <c r="F70" s="107"/>
-      <c r="G70" s="107"/>
-      <c r="H70" s="107"/>
-      <c r="I70" s="108"/>
+      <c r="B70" s="121"/>
+      <c r="C70" s="121"/>
+      <c r="D70" s="121"/>
+      <c r="E70" s="121"/>
+      <c r="F70" s="121"/>
+      <c r="G70" s="121"/>
+      <c r="H70" s="121"/>
+      <c r="I70" s="122"/>
     </row>
     <row r="71" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="109" t="s">
+      <c r="A71" s="123" t="s">
         <v>72</v>
       </c>
-      <c r="B71" s="110"/>
-      <c r="C71" s="110"/>
-      <c r="D71" s="110"/>
-      <c r="E71" s="110"/>
-      <c r="F71" s="110"/>
-      <c r="G71" s="110"/>
-      <c r="H71" s="110"/>
-      <c r="I71" s="111"/>
+      <c r="B71" s="124"/>
+      <c r="C71" s="124"/>
+      <c r="D71" s="124"/>
+      <c r="E71" s="124"/>
+      <c r="F71" s="124"/>
+      <c r="G71" s="124"/>
+      <c r="H71" s="124"/>
+      <c r="I71" s="125"/>
     </row>
     <row r="72" spans="1:9" s="52" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="95"/>
-      <c r="B72" s="95"/>
-      <c r="C72" s="95"/>
-      <c r="D72" s="95"/>
-      <c r="E72" s="95"/>
-      <c r="F72" s="95"/>
-      <c r="G72" s="95"/>
-      <c r="H72" s="95"/>
-      <c r="I72" s="95"/>
+      <c r="A72" s="109"/>
+      <c r="B72" s="109"/>
+      <c r="C72" s="109"/>
+      <c r="D72" s="109"/>
+      <c r="E72" s="109"/>
+      <c r="F72" s="109"/>
+      <c r="G72" s="109"/>
+      <c r="H72" s="109"/>
+      <c r="I72" s="109"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:I5"/>
     <mergeCell ref="K43:L43"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="C51:D51"/>
@@ -11573,13 +11580,6 @@
     <mergeCell ref="A70:I70"/>
     <mergeCell ref="A71:I71"/>
     <mergeCell ref="B52:I52"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="C31:F31"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated special leave benefit for women to match excel template
</commit_message>
<xml_diff>
--- a/templates/leave-form-template2.xlsx
+++ b/templates/leave-form-template2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Management System\backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B823D42E-BC54-4367-8677-3885942EAA8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A081EE-F59D-4679-A596-85C3D8520B52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -947,7 +947,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1093,79 +1093,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1240,6 +1189,18 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1264,35 +1225,72 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2854,8 +2852,8 @@
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>171879</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
@@ -2921,8 +2919,8 @@
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>171879</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -3323,8 +3321,8 @@
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>171879</xdr:colOff>
           <xdr:row>29</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -3390,8 +3388,8 @@
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>171879</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
@@ -8715,8 +8713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="133" zoomScaleNormal="100" zoomScaleSheetLayoutView="126" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="133" zoomScaleNormal="100" zoomScaleSheetLayoutView="126" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27:M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8737,54 +8735,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
       <c r="J1" s="53"/>
       <c r="K1" s="53"/>
       <c r="L1" s="55"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="136"/>
-      <c r="B2" s="136"/>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="136"/>
-      <c r="M2" s="136"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="137"/>
-      <c r="C3" s="137"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
-      <c r="J3" s="137"/>
-      <c r="K3" s="137"/>
-      <c r="L3" s="137"/>
-      <c r="M3" s="137"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8816,20 +8814,20 @@
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="138" t="s">
+      <c r="B5" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
       <c r="E5" s="54"/>
-      <c r="F5" s="140"/>
-      <c r="G5" s="140"/>
-      <c r="H5" s="140"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
       <c r="I5" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="J5" s="140"/>
-      <c r="K5" s="140"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
       <c r="L5" s="66"/>
       <c r="M5" s="65"/>
     </row>
@@ -8837,24 +8835,24 @@
       <c r="A6" s="62">
         <v>3</v>
       </c>
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="119" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="90"/>
+      <c r="C6" s="119"/>
       <c r="D6" s="67"/>
       <c r="E6" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="134"/>
-      <c r="G6" s="134"/>
-      <c r="H6" s="134"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="129"/>
       <c r="I6" s="5"/>
       <c r="J6" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="K6" s="100"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="101"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="128"/>
     </row>
     <row r="7" spans="1:15" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
@@ -8873,20 +8871,20 @@
     </row>
     <row r="8" spans="1:15" s="16" customFormat="1" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
-      <c r="B8" s="96" t="s">
+      <c r="B8" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="96"/>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
-      <c r="M8" s="97"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="103"/>
+      <c r="K8" s="103"/>
+      <c r="L8" s="103"/>
+      <c r="M8" s="104"/>
     </row>
     <row r="9" spans="1:15" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
@@ -8934,14 +8932,14 @@
       <c r="E11" s="21"/>
       <c r="F11" s="22"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="94" t="s">
+      <c r="H11" s="123" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="94"/>
-      <c r="J11" s="94"/>
-      <c r="K11" s="94"/>
-      <c r="L11" s="94"/>
-      <c r="M11" s="95"/>
+      <c r="I11" s="123"/>
+      <c r="J11" s="123"/>
+      <c r="K11" s="123"/>
+      <c r="L11" s="123"/>
+      <c r="M11" s="124"/>
     </row>
     <row r="12" spans="1:15" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
@@ -8976,8 +8974,8 @@
       </c>
       <c r="J13" s="60"/>
       <c r="K13" s="60"/>
-      <c r="L13" s="69"/>
-      <c r="M13" s="70"/>
+      <c r="L13" s="138"/>
+      <c r="M13" s="139"/>
     </row>
     <row r="14" spans="1:15" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
@@ -9007,13 +9005,13 @@
       <c r="F15" s="22"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="71" t="s">
+      <c r="I15" s="69" t="s">
         <v>87</v>
       </c>
       <c r="J15" s="61"/>
       <c r="K15" s="61"/>
-      <c r="L15" s="72"/>
-      <c r="M15" s="73"/>
+      <c r="L15" s="138"/>
+      <c r="M15" s="139"/>
     </row>
     <row r="16" spans="1:15" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
@@ -9040,14 +9038,14 @@
       <c r="E17" s="21"/>
       <c r="F17" s="22"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="94" t="s">
+      <c r="H17" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="94"/>
-      <c r="J17" s="94"/>
-      <c r="K17" s="94"/>
-      <c r="L17" s="94"/>
-      <c r="M17" s="95"/>
+      <c r="I17" s="123"/>
+      <c r="J17" s="123"/>
+      <c r="K17" s="123"/>
+      <c r="L17" s="123"/>
+      <c r="M17" s="124"/>
     </row>
     <row r="18" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
@@ -9074,13 +9072,13 @@
       <c r="F19" s="22"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="71" t="s">
+      <c r="I19" s="69" t="s">
         <v>88</v>
       </c>
       <c r="J19" s="61"/>
       <c r="K19" s="61"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="73"/>
+      <c r="L19" s="138"/>
+      <c r="M19" s="139"/>
     </row>
     <row r="20" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
@@ -9109,16 +9107,14 @@
       <c r="E21" s="21"/>
       <c r="F21" s="22"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" s="71" t="s">
+      <c r="H21" s="2"/>
+      <c r="I21" s="69" t="s">
         <v>89</v>
       </c>
       <c r="J21" s="61"/>
       <c r="K21" s="61"/>
-      <c r="L21" s="72"/>
-      <c r="M21" s="73"/>
+      <c r="L21" s="138"/>
+      <c r="M21" s="139"/>
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9178,14 +9174,14 @@
       <c r="E25" s="21"/>
       <c r="F25" s="22"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="94" t="s">
+      <c r="H25" s="123" t="s">
         <v>25</v>
       </c>
-      <c r="I25" s="94"/>
-      <c r="J25" s="94"/>
-      <c r="K25" s="94"/>
-      <c r="L25" s="94"/>
-      <c r="M25" s="95"/>
+      <c r="I25" s="123"/>
+      <c r="J25" s="123"/>
+      <c r="K25" s="123"/>
+      <c r="L25" s="123"/>
+      <c r="M25" s="124"/>
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9214,14 +9210,14 @@
       <c r="E27" s="21"/>
       <c r="F27" s="22"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="74" t="s">
+      <c r="H27" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="I27" s="75"/>
-      <c r="J27" s="75"/>
-      <c r="K27" s="77"/>
-      <c r="L27" s="77"/>
-      <c r="M27" s="78"/>
+      <c r="I27" s="71"/>
+      <c r="J27" s="71"/>
+      <c r="K27" s="140"/>
+      <c r="L27" s="140"/>
+      <c r="M27" s="141"/>
       <c r="N27" s="2"/>
     </row>
     <row r="28" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9267,21 +9263,21 @@
     <row r="31" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="98" t="s">
+      <c r="C31" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="98"/>
-      <c r="E31" s="98"/>
-      <c r="F31" s="99"/>
+      <c r="D31" s="125"/>
+      <c r="E31" s="125"/>
+      <c r="F31" s="126"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="94" t="s">
+      <c r="H31" s="123" t="s">
         <v>30</v>
       </c>
-      <c r="I31" s="94"/>
-      <c r="J31" s="94"/>
-      <c r="K31" s="94"/>
-      <c r="L31" s="94"/>
-      <c r="M31" s="95"/>
+      <c r="I31" s="123"/>
+      <c r="J31" s="123"/>
+      <c r="K31" s="123"/>
+      <c r="L31" s="123"/>
+      <c r="M31" s="124"/>
       <c r="N31" s="2"/>
     </row>
     <row r="32" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9311,13 +9307,13 @@
       <c r="F33" s="22"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
-      <c r="I33" s="88" t="s">
+      <c r="I33" s="105" t="s">
         <v>32</v>
       </c>
-      <c r="J33" s="88"/>
-      <c r="K33" s="88"/>
-      <c r="L33" s="88"/>
-      <c r="M33" s="89"/>
+      <c r="J33" s="105"/>
+      <c r="K33" s="105"/>
+      <c r="L33" s="105"/>
+      <c r="M33" s="106"/>
       <c r="N33" s="2"/>
     </row>
     <row r="34" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9346,13 +9342,13 @@
       <c r="F35" s="14"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
-      <c r="I35" s="88" t="s">
+      <c r="I35" s="105" t="s">
         <v>34</v>
       </c>
-      <c r="J35" s="88"/>
-      <c r="K35" s="88"/>
-      <c r="L35" s="88"/>
-      <c r="M35" s="89"/>
+      <c r="J35" s="105"/>
+      <c r="K35" s="105"/>
+      <c r="L35" s="105"/>
+      <c r="M35" s="106"/>
     </row>
     <row r="36" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
@@ -9373,14 +9369,14 @@
       <c r="E37" s="2"/>
       <c r="F37" s="14"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="86" t="s">
+      <c r="H37" s="117" t="s">
         <v>35</v>
       </c>
-      <c r="I37" s="86"/>
-      <c r="J37" s="86"/>
-      <c r="K37" s="86"/>
-      <c r="L37" s="86"/>
-      <c r="M37" s="87"/>
+      <c r="I37" s="117"/>
+      <c r="J37" s="117"/>
+      <c r="K37" s="117"/>
+      <c r="L37" s="117"/>
+      <c r="M37" s="118"/>
     </row>
     <row r="38" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
@@ -9407,16 +9403,14 @@
       <c r="E39" s="2"/>
       <c r="F39" s="14"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I39" s="88" t="s">
+      <c r="H39" s="2"/>
+      <c r="I39" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="J39" s="88"/>
-      <c r="K39" s="88"/>
-      <c r="L39" s="88"/>
-      <c r="M39" s="89"/>
+      <c r="J39" s="105"/>
+      <c r="K39" s="105"/>
+      <c r="L39" s="105"/>
+      <c r="M39" s="106"/>
     </row>
     <row r="40" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
@@ -9443,16 +9437,14 @@
       <c r="E41" s="2"/>
       <c r="F41" s="14"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I41" s="88" t="s">
+      <c r="H41" s="2"/>
+      <c r="I41" s="105" t="s">
         <v>39</v>
       </c>
-      <c r="J41" s="88"/>
-      <c r="K41" s="88"/>
-      <c r="L41" s="88"/>
-      <c r="M41" s="89"/>
+      <c r="J41" s="105"/>
+      <c r="K41" s="105"/>
+      <c r="L41" s="105"/>
+      <c r="M41" s="106"/>
     </row>
     <row r="42" spans="1:16" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
@@ -9483,8 +9475,8 @@
       </c>
       <c r="H43" s="30"/>
       <c r="M43" s="26"/>
-      <c r="O43" s="102"/>
-      <c r="P43" s="103"/>
+      <c r="O43" s="79"/>
+      <c r="P43" s="80"/>
     </row>
     <row r="44" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="29"/>
@@ -9499,20 +9491,20 @@
     </row>
     <row r="45" spans="1:16" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
-      <c r="B45" s="93"/>
-      <c r="C45" s="93"/>
-      <c r="D45" s="93"/>
-      <c r="E45" s="93"/>
+      <c r="B45" s="122"/>
+      <c r="C45" s="122"/>
+      <c r="D45" s="122"/>
+      <c r="E45" s="122"/>
       <c r="F45" s="14"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
-      <c r="I45" s="91" t="s">
+      <c r="I45" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="J45" s="91"/>
-      <c r="K45" s="91"/>
-      <c r="L45" s="91"/>
-      <c r="M45" s="92"/>
+      <c r="J45" s="120"/>
+      <c r="K45" s="120"/>
+      <c r="L45" s="120"/>
+      <c r="M45" s="121"/>
     </row>
     <row r="46" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
@@ -9540,19 +9532,19 @@
       <c r="F47" s="14"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
-      <c r="I47" s="88" t="s">
+      <c r="I47" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="J47" s="88"/>
-      <c r="K47" s="88"/>
-      <c r="L47" s="88"/>
-      <c r="M47" s="89"/>
+      <c r="J47" s="105"/>
+      <c r="K47" s="105"/>
+      <c r="L47" s="105"/>
+      <c r="M47" s="106"/>
     </row>
     <row r="48" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="31"/>
-      <c r="C48" s="104"/>
-      <c r="D48" s="105"/>
+      <c r="C48" s="81"/>
+      <c r="D48" s="82"/>
       <c r="E48" s="2"/>
       <c r="F48" s="14"/>
       <c r="G48" s="2"/>
@@ -9580,58 +9572,58 @@
     </row>
     <row r="50" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11"/>
-      <c r="B50" s="129" t="s">
+      <c r="B50" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="130"/>
-      <c r="D50" s="130"/>
-      <c r="E50" s="130"/>
+      <c r="C50" s="111"/>
+      <c r="D50" s="111"/>
+      <c r="E50" s="111"/>
       <c r="F50" s="14"/>
-      <c r="G50" s="126" t="s">
+      <c r="G50" s="107" t="s">
         <v>83</v>
       </c>
-      <c r="H50" s="127"/>
-      <c r="I50" s="127"/>
-      <c r="J50" s="127"/>
-      <c r="K50" s="127"/>
-      <c r="L50" s="127"/>
-      <c r="M50" s="128"/>
+      <c r="H50" s="108"/>
+      <c r="I50" s="108"/>
+      <c r="J50" s="108"/>
+      <c r="K50" s="108"/>
+      <c r="L50" s="108"/>
+      <c r="M50" s="109"/>
     </row>
     <row r="51" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="131" t="s">
+      <c r="A51" s="112" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="132"/>
-      <c r="C51" s="132"/>
-      <c r="D51" s="132"/>
-      <c r="E51" s="132"/>
-      <c r="F51" s="133"/>
-      <c r="G51" s="106" t="s">
+      <c r="B51" s="113"/>
+      <c r="C51" s="113"/>
+      <c r="D51" s="113"/>
+      <c r="E51" s="113"/>
+      <c r="F51" s="114"/>
+      <c r="G51" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="H51" s="107"/>
-      <c r="I51" s="107"/>
-      <c r="J51" s="107"/>
-      <c r="K51" s="107"/>
-      <c r="L51" s="107"/>
-      <c r="M51" s="108"/>
+      <c r="H51" s="84"/>
+      <c r="I51" s="84"/>
+      <c r="J51" s="84"/>
+      <c r="K51" s="84"/>
+      <c r="L51" s="84"/>
+      <c r="M51" s="85"/>
     </row>
     <row r="52" spans="1:13" s="16" customFormat="1" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
-      <c r="B52" s="96" t="s">
+      <c r="B52" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="96"/>
-      <c r="D52" s="96"/>
-      <c r="E52" s="96"/>
-      <c r="F52" s="96"/>
-      <c r="G52" s="96"/>
-      <c r="H52" s="96"/>
-      <c r="I52" s="96"/>
-      <c r="J52" s="96"/>
-      <c r="K52" s="96"/>
-      <c r="L52" s="96"/>
-      <c r="M52" s="97"/>
+      <c r="C52" s="103"/>
+      <c r="D52" s="103"/>
+      <c r="E52" s="103"/>
+      <c r="F52" s="103"/>
+      <c r="G52" s="103"/>
+      <c r="H52" s="103"/>
+      <c r="I52" s="103"/>
+      <c r="J52" s="103"/>
+      <c r="K52" s="103"/>
+      <c r="L52" s="103"/>
+      <c r="M52" s="104"/>
     </row>
     <row r="53" spans="1:13" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
@@ -9677,13 +9669,13 @@
       <c r="F55" s="14"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
-      <c r="I55" s="84" t="s">
+      <c r="I55" s="115" t="s">
         <v>53</v>
       </c>
-      <c r="J55" s="84"/>
-      <c r="K55" s="84"/>
-      <c r="L55" s="84"/>
-      <c r="M55" s="85"/>
+      <c r="J55" s="115"/>
+      <c r="K55" s="115"/>
+      <c r="L55" s="115"/>
+      <c r="M55" s="116"/>
     </row>
     <row r="56" spans="1:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11"/>
@@ -9713,13 +9705,13 @@
       <c r="F57" s="14"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
-      <c r="I57" s="75" t="s">
+      <c r="I57" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="J57" s="75"/>
-      <c r="K57" s="75"/>
-      <c r="L57" s="75"/>
-      <c r="M57" s="76"/>
+      <c r="J57" s="71"/>
+      <c r="K57" s="71"/>
+      <c r="L57" s="71"/>
+      <c r="M57" s="72"/>
     </row>
     <row r="58" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="11"/>
@@ -9732,13 +9724,13 @@
       <c r="F58" s="14"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
-      <c r="I58" s="84" t="s">
+      <c r="I58" s="115" t="s">
         <v>58</v>
       </c>
-      <c r="J58" s="84"/>
-      <c r="K58" s="84"/>
-      <c r="L58" s="84"/>
-      <c r="M58" s="85"/>
+      <c r="J58" s="115"/>
+      <c r="K58" s="115"/>
+      <c r="L58" s="115"/>
+      <c r="M58" s="116"/>
     </row>
     <row r="59" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11"/>
@@ -9751,13 +9743,13 @@
       <c r="F59" s="14"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
-      <c r="I59" s="84" t="s">
+      <c r="I59" s="115" t="s">
         <v>58</v>
       </c>
-      <c r="J59" s="84"/>
-      <c r="K59" s="84"/>
-      <c r="L59" s="84"/>
-      <c r="M59" s="85"/>
+      <c r="J59" s="115"/>
+      <c r="K59" s="115"/>
+      <c r="L59" s="115"/>
+      <c r="M59" s="116"/>
     </row>
     <row r="60" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="11"/>
@@ -9770,44 +9762,44 @@
       <c r="F60" s="14"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
-      <c r="I60" s="84" t="s">
+      <c r="I60" s="115" t="s">
         <v>58</v>
       </c>
-      <c r="J60" s="84"/>
-      <c r="K60" s="84"/>
-      <c r="L60" s="84"/>
-      <c r="M60" s="85"/>
+      <c r="J60" s="115"/>
+      <c r="K60" s="115"/>
+      <c r="L60" s="115"/>
+      <c r="M60" s="116"/>
     </row>
     <row r="61" spans="1:13" s="45" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="44"/>
-      <c r="G61" s="79" t="s">
+      <c r="G61" s="130" t="s">
         <v>61</v>
       </c>
-      <c r="H61" s="80"/>
-      <c r="I61" s="80"/>
-      <c r="J61" s="80"/>
-      <c r="K61" s="80"/>
-      <c r="L61" s="80"/>
-      <c r="M61" s="81"/>
+      <c r="H61" s="131"/>
+      <c r="I61" s="131"/>
+      <c r="J61" s="131"/>
+      <c r="K61" s="131"/>
+      <c r="L61" s="131"/>
+      <c r="M61" s="132"/>
     </row>
     <row r="62" spans="1:13" s="49" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="47"/>
       <c r="B62" s="37"/>
-      <c r="C62" s="110" t="s">
+      <c r="C62" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="D62" s="110"/>
-      <c r="E62" s="110"/>
+      <c r="D62" s="87"/>
+      <c r="E62" s="87"/>
       <c r="F62" s="48"/>
-      <c r="G62" s="111" t="s">
+      <c r="G62" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="H62" s="112"/>
-      <c r="I62" s="107"/>
-      <c r="J62" s="107"/>
-      <c r="K62" s="107"/>
-      <c r="L62" s="107"/>
-      <c r="M62" s="113"/>
+      <c r="H62" s="89"/>
+      <c r="I62" s="84"/>
+      <c r="J62" s="84"/>
+      <c r="K62" s="84"/>
+      <c r="L62" s="84"/>
+      <c r="M62" s="90"/>
     </row>
     <row r="63" spans="1:13" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
@@ -9837,14 +9829,14 @@
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="82" t="s">
+      <c r="H64" s="133" t="s">
         <v>66</v>
       </c>
-      <c r="I64" s="82"/>
-      <c r="J64" s="82"/>
-      <c r="K64" s="82"/>
-      <c r="L64" s="82"/>
-      <c r="M64" s="83"/>
+      <c r="I64" s="133"/>
+      <c r="J64" s="133"/>
+      <c r="K64" s="133"/>
+      <c r="L64" s="133"/>
+      <c r="M64" s="134"/>
     </row>
     <row r="65" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="11"/>
@@ -9855,14 +9847,14 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="H65" s="84" t="s">
+      <c r="H65" s="115" t="s">
         <v>58</v>
       </c>
-      <c r="I65" s="84"/>
-      <c r="J65" s="84"/>
-      <c r="K65" s="84"/>
-      <c r="L65" s="84"/>
-      <c r="M65" s="85"/>
+      <c r="I65" s="115"/>
+      <c r="J65" s="115"/>
+      <c r="K65" s="115"/>
+      <c r="L65" s="115"/>
+      <c r="M65" s="116"/>
     </row>
     <row r="66" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="11"/>
@@ -9873,14 +9865,14 @@
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-      <c r="H66" s="84" t="s">
+      <c r="H66" s="115" t="s">
         <v>58</v>
       </c>
-      <c r="I66" s="84"/>
-      <c r="J66" s="84"/>
-      <c r="K66" s="84"/>
-      <c r="L66" s="84"/>
-      <c r="M66" s="85"/>
+      <c r="I66" s="115"/>
+      <c r="J66" s="115"/>
+      <c r="K66" s="115"/>
+      <c r="L66" s="115"/>
+      <c r="M66" s="116"/>
     </row>
     <row r="67" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="11"/>
@@ -9897,96 +9889,118 @@
       <c r="M67" s="14"/>
     </row>
     <row r="68" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="114" t="s">
+      <c r="A68" s="91" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="115"/>
-      <c r="C68" s="115"/>
-      <c r="D68" s="115"/>
-      <c r="E68" s="115"/>
-      <c r="F68" s="115"/>
-      <c r="G68" s="115"/>
-      <c r="H68" s="115"/>
-      <c r="I68" s="115"/>
-      <c r="J68" s="115"/>
-      <c r="K68" s="115"/>
-      <c r="L68" s="115"/>
-      <c r="M68" s="116"/>
+      <c r="B68" s="92"/>
+      <c r="C68" s="92"/>
+      <c r="D68" s="92"/>
+      <c r="E68" s="92"/>
+      <c r="F68" s="92"/>
+      <c r="G68" s="92"/>
+      <c r="H68" s="92"/>
+      <c r="I68" s="92"/>
+      <c r="J68" s="92"/>
+      <c r="K68" s="92"/>
+      <c r="L68" s="92"/>
+      <c r="M68" s="93"/>
     </row>
     <row r="69" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="117" t="s">
+      <c r="A69" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="118"/>
-      <c r="C69" s="118"/>
-      <c r="D69" s="118"/>
-      <c r="E69" s="118"/>
-      <c r="F69" s="118"/>
-      <c r="G69" s="118"/>
-      <c r="H69" s="118"/>
-      <c r="I69" s="118"/>
-      <c r="J69" s="118"/>
-      <c r="K69" s="118"/>
-      <c r="L69" s="118"/>
-      <c r="M69" s="119"/>
+      <c r="B69" s="95"/>
+      <c r="C69" s="95"/>
+      <c r="D69" s="95"/>
+      <c r="E69" s="95"/>
+      <c r="F69" s="95"/>
+      <c r="G69" s="95"/>
+      <c r="H69" s="95"/>
+      <c r="I69" s="95"/>
+      <c r="J69" s="95"/>
+      <c r="K69" s="95"/>
+      <c r="L69" s="95"/>
+      <c r="M69" s="96"/>
     </row>
     <row r="70" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="120" t="s">
+      <c r="A70" s="97" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="121"/>
-      <c r="C70" s="121"/>
-      <c r="D70" s="121"/>
-      <c r="E70" s="121"/>
-      <c r="F70" s="121"/>
-      <c r="G70" s="121"/>
-      <c r="H70" s="121"/>
-      <c r="I70" s="121"/>
-      <c r="J70" s="121"/>
-      <c r="K70" s="121"/>
-      <c r="L70" s="121"/>
-      <c r="M70" s="122"/>
+      <c r="B70" s="98"/>
+      <c r="C70" s="98"/>
+      <c r="D70" s="98"/>
+      <c r="E70" s="98"/>
+      <c r="F70" s="98"/>
+      <c r="G70" s="98"/>
+      <c r="H70" s="98"/>
+      <c r="I70" s="98"/>
+      <c r="J70" s="98"/>
+      <c r="K70" s="98"/>
+      <c r="L70" s="98"/>
+      <c r="M70" s="99"/>
     </row>
     <row r="71" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="123" t="s">
+      <c r="A71" s="100" t="s">
         <v>72</v>
       </c>
-      <c r="B71" s="124"/>
-      <c r="C71" s="124"/>
-      <c r="D71" s="124"/>
-      <c r="E71" s="124"/>
-      <c r="F71" s="124"/>
-      <c r="G71" s="124"/>
-      <c r="H71" s="124"/>
-      <c r="I71" s="124"/>
-      <c r="J71" s="124"/>
-      <c r="K71" s="124"/>
-      <c r="L71" s="124"/>
-      <c r="M71" s="125"/>
+      <c r="B71" s="101"/>
+      <c r="C71" s="101"/>
+      <c r="D71" s="101"/>
+      <c r="E71" s="101"/>
+      <c r="F71" s="101"/>
+      <c r="G71" s="101"/>
+      <c r="H71" s="101"/>
+      <c r="I71" s="101"/>
+      <c r="J71" s="101"/>
+      <c r="K71" s="101"/>
+      <c r="L71" s="101"/>
+      <c r="M71" s="102"/>
     </row>
     <row r="72" spans="1:13" s="52" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="109"/>
-      <c r="B72" s="109"/>
-      <c r="C72" s="109"/>
-      <c r="D72" s="109"/>
-      <c r="E72" s="109"/>
-      <c r="F72" s="109"/>
-      <c r="G72" s="109"/>
-      <c r="H72" s="109"/>
-      <c r="I72" s="109"/>
-      <c r="J72" s="109"/>
-      <c r="K72" s="109"/>
-      <c r="L72" s="109"/>
-      <c r="M72" s="109"/>
+      <c r="A72" s="86"/>
+      <c r="B72" s="86"/>
+      <c r="C72" s="86"/>
+      <c r="D72" s="86"/>
+      <c r="E72" s="86"/>
+      <c r="F72" s="86"/>
+      <c r="G72" s="86"/>
+      <c r="H72" s="86"/>
+      <c r="I72" s="86"/>
+      <c r="J72" s="86"/>
+      <c r="K72" s="86"/>
+      <c r="L72" s="86"/>
+      <c r="M72" s="86"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="J5:K5"/>
+  <mergeCells count="50">
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="G61:M61"/>
+    <mergeCell ref="H64:M64"/>
+    <mergeCell ref="H65:M65"/>
+    <mergeCell ref="H66:M66"/>
+    <mergeCell ref="I58:M58"/>
+    <mergeCell ref="I59:M59"/>
+    <mergeCell ref="I60:M60"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="I41:M41"/>
+    <mergeCell ref="I39:M39"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="I45:M45"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="I35:M35"/>
+    <mergeCell ref="I33:M33"/>
+    <mergeCell ref="B8:M8"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H17:M17"/>
     <mergeCell ref="O43:P43"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="G51:M51"/>
@@ -10003,29 +10017,12 @@
     <mergeCell ref="B50:E50"/>
     <mergeCell ref="A51:F51"/>
     <mergeCell ref="I55:M55"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="I41:M41"/>
-    <mergeCell ref="I39:M39"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="I45:M45"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="I35:M35"/>
-    <mergeCell ref="I33:M33"/>
-    <mergeCell ref="B8:M8"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="G61:M61"/>
-    <mergeCell ref="H64:M64"/>
-    <mergeCell ref="H65:M65"/>
-    <mergeCell ref="H66:M66"/>
-    <mergeCell ref="I58:M58"/>
-    <mergeCell ref="I59:M59"/>
-    <mergeCell ref="I60:M60"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="J5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10612,42 +10609,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="136"/>
-      <c r="B2" s="136"/>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="137"/>
-      <c r="C3" s="137"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -10669,14 +10666,14 @@
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="142"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="139"/>
-      <c r="I5" s="143"/>
+      <c r="B5" s="135"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="136"/>
     </row>
     <row r="6" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
@@ -10705,16 +10702,16 @@
     </row>
     <row r="8" spans="1:11" s="16" customFormat="1" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
-      <c r="B8" s="96" t="s">
+      <c r="B8" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="97"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="104"/>
     </row>
     <row r="9" spans="1:11" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
@@ -11007,12 +11004,12 @@
     <row r="31" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="98" t="s">
+      <c r="C31" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="98"/>
-      <c r="E31" s="98"/>
-      <c r="F31" s="99"/>
+      <c r="D31" s="125"/>
+      <c r="E31" s="125"/>
+      <c r="F31" s="126"/>
       <c r="G31" s="2"/>
       <c r="H31" s="23" t="s">
         <v>30</v>
@@ -11173,8 +11170,8 @@
         <v>41</v>
       </c>
       <c r="I43" s="26"/>
-      <c r="K43" s="102"/>
-      <c r="L43" s="103"/>
+      <c r="K43" s="79"/>
+      <c r="L43" s="80"/>
     </row>
     <row r="44" spans="1:12" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="29"/>
@@ -11230,8 +11227,8 @@
     <row r="48" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
       <c r="B48" s="31"/>
-      <c r="C48" s="102"/>
-      <c r="D48" s="103"/>
+      <c r="C48" s="79"/>
+      <c r="D48" s="80"/>
       <c r="E48" s="2"/>
       <c r="F48" s="14"/>
       <c r="G48" s="2"/>
@@ -11269,30 +11266,30 @@
         <v>47</v>
       </c>
       <c r="B51" s="2"/>
-      <c r="C51" s="112" t="s">
+      <c r="C51" s="89" t="s">
         <v>73</v>
       </c>
-      <c r="D51" s="107"/>
+      <c r="D51" s="84"/>
       <c r="E51" s="37"/>
       <c r="F51" s="14"/>
-      <c r="G51" s="141" t="s">
+      <c r="G51" s="137" t="s">
         <v>48</v>
       </c>
-      <c r="H51" s="107"/>
-      <c r="I51" s="108"/>
+      <c r="H51" s="84"/>
+      <c r="I51" s="85"/>
     </row>
     <row r="52" spans="1:9" s="16" customFormat="1" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
-      <c r="B52" s="96" t="s">
+      <c r="B52" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="96"/>
-      <c r="D52" s="96"/>
-      <c r="E52" s="96"/>
-      <c r="F52" s="96"/>
-      <c r="G52" s="96"/>
-      <c r="H52" s="96"/>
-      <c r="I52" s="97"/>
+      <c r="C52" s="103"/>
+      <c r="D52" s="103"/>
+      <c r="E52" s="103"/>
+      <c r="F52" s="103"/>
+      <c r="G52" s="103"/>
+      <c r="H52" s="103"/>
+      <c r="I52" s="104"/>
     </row>
     <row r="53" spans="1:9" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
@@ -11417,17 +11414,17 @@
     <row r="62" spans="1:9" s="49" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="47"/>
       <c r="B62" s="37"/>
-      <c r="C62" s="110" t="s">
+      <c r="C62" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="D62" s="110"/>
-      <c r="E62" s="110"/>
+      <c r="D62" s="87"/>
+      <c r="E62" s="87"/>
       <c r="F62" s="48"/>
-      <c r="G62" s="111" t="s">
+      <c r="G62" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="H62" s="107"/>
-      <c r="I62" s="113"/>
+      <c r="H62" s="84"/>
+      <c r="I62" s="90"/>
     </row>
     <row r="63" spans="1:9" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
@@ -11497,77 +11494,70 @@
       <c r="I67" s="14"/>
     </row>
     <row r="68" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="114" t="s">
+      <c r="A68" s="91" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="115"/>
-      <c r="C68" s="115"/>
-      <c r="D68" s="115"/>
-      <c r="E68" s="115"/>
-      <c r="F68" s="115"/>
-      <c r="G68" s="115"/>
-      <c r="H68" s="115"/>
-      <c r="I68" s="116"/>
+      <c r="B68" s="92"/>
+      <c r="C68" s="92"/>
+      <c r="D68" s="92"/>
+      <c r="E68" s="92"/>
+      <c r="F68" s="92"/>
+      <c r="G68" s="92"/>
+      <c r="H68" s="92"/>
+      <c r="I68" s="93"/>
     </row>
     <row r="69" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="117" t="s">
+      <c r="A69" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="118"/>
-      <c r="C69" s="118"/>
-      <c r="D69" s="118"/>
-      <c r="E69" s="118"/>
-      <c r="F69" s="118"/>
-      <c r="G69" s="118"/>
-      <c r="H69" s="118"/>
-      <c r="I69" s="119"/>
+      <c r="B69" s="95"/>
+      <c r="C69" s="95"/>
+      <c r="D69" s="95"/>
+      <c r="E69" s="95"/>
+      <c r="F69" s="95"/>
+      <c r="G69" s="95"/>
+      <c r="H69" s="95"/>
+      <c r="I69" s="96"/>
     </row>
     <row r="70" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="120" t="s">
+      <c r="A70" s="97" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="121"/>
-      <c r="C70" s="121"/>
-      <c r="D70" s="121"/>
-      <c r="E70" s="121"/>
-      <c r="F70" s="121"/>
-      <c r="G70" s="121"/>
-      <c r="H70" s="121"/>
-      <c r="I70" s="122"/>
+      <c r="B70" s="98"/>
+      <c r="C70" s="98"/>
+      <c r="D70" s="98"/>
+      <c r="E70" s="98"/>
+      <c r="F70" s="98"/>
+      <c r="G70" s="98"/>
+      <c r="H70" s="98"/>
+      <c r="I70" s="99"/>
     </row>
     <row r="71" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="123" t="s">
+      <c r="A71" s="100" t="s">
         <v>72</v>
       </c>
-      <c r="B71" s="124"/>
-      <c r="C71" s="124"/>
-      <c r="D71" s="124"/>
-      <c r="E71" s="124"/>
-      <c r="F71" s="124"/>
-      <c r="G71" s="124"/>
-      <c r="H71" s="124"/>
-      <c r="I71" s="125"/>
+      <c r="B71" s="101"/>
+      <c r="C71" s="101"/>
+      <c r="D71" s="101"/>
+      <c r="E71" s="101"/>
+      <c r="F71" s="101"/>
+      <c r="G71" s="101"/>
+      <c r="H71" s="101"/>
+      <c r="I71" s="102"/>
     </row>
     <row r="72" spans="1:9" s="52" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="109"/>
-      <c r="B72" s="109"/>
-      <c r="C72" s="109"/>
-      <c r="D72" s="109"/>
-      <c r="E72" s="109"/>
-      <c r="F72" s="109"/>
-      <c r="G72" s="109"/>
-      <c r="H72" s="109"/>
-      <c r="I72" s="109"/>
+      <c r="A72" s="86"/>
+      <c r="B72" s="86"/>
+      <c r="C72" s="86"/>
+      <c r="D72" s="86"/>
+      <c r="E72" s="86"/>
+      <c r="F72" s="86"/>
+      <c r="G72" s="86"/>
+      <c r="H72" s="86"/>
+      <c r="I72" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:I5"/>
     <mergeCell ref="K43:L43"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="C51:D51"/>
@@ -11580,6 +11570,13 @@
     <mergeCell ref="A70:I70"/>
     <mergeCell ref="A71:I71"/>
     <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:I5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added template data for excel file
</commit_message>
<xml_diff>
--- a/templates/leave-form-template2.xlsx
+++ b/templates/leave-form-template2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Management System\backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A081EE-F59D-4679-A596-85C3D8520B52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E7DD9B-5674-4054-965E-D6BC638DF9C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1099,22 +1099,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1189,18 +1241,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1225,72 +1265,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2852,8 +2852,8 @@
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>171879</xdr:colOff>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
@@ -2919,8 +2919,8 @@
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>171879</xdr:colOff>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -3321,8 +3321,8 @@
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>171879</xdr:colOff>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>29</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -3388,8 +3388,8 @@
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>171879</xdr:colOff>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
@@ -8713,8 +8713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="133" zoomScaleNormal="100" zoomScaleSheetLayoutView="126" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27:M27"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A32" zoomScale="133" zoomScaleNormal="100" zoomScaleSheetLayoutView="126" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8735,54 +8735,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="133" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
       <c r="J1" s="53"/>
       <c r="K1" s="53"/>
       <c r="L1" s="55"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="74"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
+      <c r="A2" s="134"/>
+      <c r="B2" s="134"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="135" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="75"/>
+      <c r="B3" s="135"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="135"/>
+      <c r="G3" s="135"/>
+      <c r="H3" s="135"/>
+      <c r="I3" s="135"/>
+      <c r="J3" s="135"/>
+      <c r="K3" s="135"/>
+      <c r="L3" s="135"/>
+      <c r="M3" s="135"/>
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8814,20 +8814,20 @@
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="136" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
+      <c r="C5" s="137"/>
+      <c r="D5" s="137"/>
       <c r="E5" s="54"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
+      <c r="F5" s="138"/>
+      <c r="G5" s="138"/>
+      <c r="H5" s="138"/>
       <c r="I5" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
+      <c r="J5" s="138"/>
+      <c r="K5" s="138"/>
       <c r="L5" s="66"/>
       <c r="M5" s="65"/>
     </row>
@@ -8835,24 +8835,24 @@
       <c r="A6" s="62">
         <v>3</v>
       </c>
-      <c r="B6" s="119" t="s">
+      <c r="B6" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="119"/>
+      <c r="C6" s="88"/>
       <c r="D6" s="67"/>
       <c r="E6" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="129"/>
-      <c r="G6" s="129"/>
-      <c r="H6" s="129"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
       <c r="I6" s="5"/>
       <c r="J6" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="K6" s="127"/>
-      <c r="L6" s="127"/>
-      <c r="M6" s="128"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="99"/>
     </row>
     <row r="7" spans="1:15" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
@@ -8871,20 +8871,20 @@
     </row>
     <row r="8" spans="1:15" s="16" customFormat="1" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="103"/>
-      <c r="F8" s="103"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="103"/>
-      <c r="J8" s="103"/>
-      <c r="K8" s="103"/>
-      <c r="L8" s="103"/>
-      <c r="M8" s="104"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
+      <c r="M8" s="95"/>
     </row>
     <row r="9" spans="1:15" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
@@ -8932,14 +8932,14 @@
       <c r="E11" s="21"/>
       <c r="F11" s="22"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="123" t="s">
+      <c r="H11" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="123"/>
-      <c r="J11" s="123"/>
-      <c r="K11" s="123"/>
-      <c r="L11" s="123"/>
-      <c r="M11" s="124"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="92"/>
+      <c r="K11" s="92"/>
+      <c r="L11" s="92"/>
+      <c r="M11" s="93"/>
     </row>
     <row r="12" spans="1:15" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
@@ -8974,8 +8974,8 @@
       </c>
       <c r="J13" s="60"/>
       <c r="K13" s="60"/>
-      <c r="L13" s="138"/>
-      <c r="M13" s="139"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="74"/>
     </row>
     <row r="14" spans="1:15" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
@@ -9010,8 +9010,8 @@
       </c>
       <c r="J15" s="61"/>
       <c r="K15" s="61"/>
-      <c r="L15" s="138"/>
-      <c r="M15" s="139"/>
+      <c r="L15" s="73"/>
+      <c r="M15" s="74"/>
     </row>
     <row r="16" spans="1:15" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
@@ -9038,14 +9038,14 @@
       <c r="E17" s="21"/>
       <c r="F17" s="22"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="123" t="s">
+      <c r="H17" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="123"/>
-      <c r="J17" s="123"/>
-      <c r="K17" s="123"/>
-      <c r="L17" s="123"/>
-      <c r="M17" s="124"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="93"/>
     </row>
     <row r="18" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
@@ -9077,8 +9077,8 @@
       </c>
       <c r="J19" s="61"/>
       <c r="K19" s="61"/>
-      <c r="L19" s="138"/>
-      <c r="M19" s="139"/>
+      <c r="L19" s="73"/>
+      <c r="M19" s="74"/>
     </row>
     <row r="20" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
@@ -9113,8 +9113,8 @@
       </c>
       <c r="J21" s="61"/>
       <c r="K21" s="61"/>
-      <c r="L21" s="138"/>
-      <c r="M21" s="139"/>
+      <c r="L21" s="73"/>
+      <c r="M21" s="74"/>
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9174,14 +9174,14 @@
       <c r="E25" s="21"/>
       <c r="F25" s="22"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="123" t="s">
+      <c r="H25" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="I25" s="123"/>
-      <c r="J25" s="123"/>
-      <c r="K25" s="123"/>
-      <c r="L25" s="123"/>
-      <c r="M25" s="124"/>
+      <c r="I25" s="92"/>
+      <c r="J25" s="92"/>
+      <c r="K25" s="92"/>
+      <c r="L25" s="92"/>
+      <c r="M25" s="93"/>
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9215,9 +9215,9 @@
       </c>
       <c r="I27" s="71"/>
       <c r="J27" s="71"/>
-      <c r="K27" s="140"/>
-      <c r="L27" s="140"/>
-      <c r="M27" s="141"/>
+      <c r="K27" s="75"/>
+      <c r="L27" s="75"/>
+      <c r="M27" s="76"/>
       <c r="N27" s="2"/>
     </row>
     <row r="28" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9263,21 +9263,21 @@
     <row r="31" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="125" t="s">
+      <c r="C31" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="125"/>
-      <c r="E31" s="125"/>
-      <c r="F31" s="126"/>
+      <c r="D31" s="96"/>
+      <c r="E31" s="96"/>
+      <c r="F31" s="97"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="123" t="s">
+      <c r="H31" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="I31" s="123"/>
-      <c r="J31" s="123"/>
-      <c r="K31" s="123"/>
-      <c r="L31" s="123"/>
-      <c r="M31" s="124"/>
+      <c r="I31" s="92"/>
+      <c r="J31" s="92"/>
+      <c r="K31" s="92"/>
+      <c r="L31" s="92"/>
+      <c r="M31" s="93"/>
       <c r="N31" s="2"/>
     </row>
     <row r="32" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9307,13 +9307,13 @@
       <c r="F33" s="22"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
-      <c r="I33" s="105" t="s">
+      <c r="I33" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="J33" s="105"/>
-      <c r="K33" s="105"/>
-      <c r="L33" s="105"/>
-      <c r="M33" s="106"/>
+      <c r="J33" s="86"/>
+      <c r="K33" s="86"/>
+      <c r="L33" s="86"/>
+      <c r="M33" s="87"/>
       <c r="N33" s="2"/>
     </row>
     <row r="34" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9342,13 +9342,13 @@
       <c r="F35" s="14"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
-      <c r="I35" s="105" t="s">
+      <c r="I35" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="J35" s="105"/>
-      <c r="K35" s="105"/>
-      <c r="L35" s="105"/>
-      <c r="M35" s="106"/>
+      <c r="J35" s="86"/>
+      <c r="K35" s="86"/>
+      <c r="L35" s="86"/>
+      <c r="M35" s="87"/>
     </row>
     <row r="36" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
@@ -9369,14 +9369,14 @@
       <c r="E37" s="2"/>
       <c r="F37" s="14"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="117" t="s">
+      <c r="H37" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="I37" s="117"/>
-      <c r="J37" s="117"/>
-      <c r="K37" s="117"/>
-      <c r="L37" s="117"/>
-      <c r="M37" s="118"/>
+      <c r="I37" s="84"/>
+      <c r="J37" s="84"/>
+      <c r="K37" s="84"/>
+      <c r="L37" s="84"/>
+      <c r="M37" s="85"/>
     </row>
     <row r="38" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
@@ -9404,13 +9404,13 @@
       <c r="F39" s="14"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
-      <c r="I39" s="105" t="s">
+      <c r="I39" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="J39" s="105"/>
-      <c r="K39" s="105"/>
-      <c r="L39" s="105"/>
-      <c r="M39" s="106"/>
+      <c r="J39" s="86"/>
+      <c r="K39" s="86"/>
+      <c r="L39" s="86"/>
+      <c r="M39" s="87"/>
     </row>
     <row r="40" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
@@ -9438,13 +9438,13 @@
       <c r="F41" s="14"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
-      <c r="I41" s="105" t="s">
+      <c r="I41" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="J41" s="105"/>
-      <c r="K41" s="105"/>
-      <c r="L41" s="105"/>
-      <c r="M41" s="106"/>
+      <c r="J41" s="86"/>
+      <c r="K41" s="86"/>
+      <c r="L41" s="86"/>
+      <c r="M41" s="87"/>
     </row>
     <row r="42" spans="1:16" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
@@ -9475,8 +9475,8 @@
       </c>
       <c r="H43" s="30"/>
       <c r="M43" s="26"/>
-      <c r="O43" s="79"/>
-      <c r="P43" s="80"/>
+      <c r="O43" s="101"/>
+      <c r="P43" s="102"/>
     </row>
     <row r="44" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="29"/>
@@ -9491,20 +9491,20 @@
     </row>
     <row r="45" spans="1:16" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
-      <c r="B45" s="122"/>
-      <c r="C45" s="122"/>
-      <c r="D45" s="122"/>
-      <c r="E45" s="122"/>
+      <c r="B45" s="91"/>
+      <c r="C45" s="91"/>
+      <c r="D45" s="91"/>
+      <c r="E45" s="91"/>
       <c r="F45" s="14"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
-      <c r="I45" s="120" t="s">
+      <c r="I45" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="J45" s="120"/>
-      <c r="K45" s="120"/>
-      <c r="L45" s="120"/>
-      <c r="M45" s="121"/>
+      <c r="J45" s="89"/>
+      <c r="K45" s="89"/>
+      <c r="L45" s="89"/>
+      <c r="M45" s="90"/>
     </row>
     <row r="46" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
@@ -9532,19 +9532,19 @@
       <c r="F47" s="14"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
-      <c r="I47" s="105" t="s">
+      <c r="I47" s="86" t="s">
         <v>45</v>
       </c>
-      <c r="J47" s="105"/>
-      <c r="K47" s="105"/>
-      <c r="L47" s="105"/>
-      <c r="M47" s="106"/>
+      <c r="J47" s="86"/>
+      <c r="K47" s="86"/>
+      <c r="L47" s="86"/>
+      <c r="M47" s="87"/>
     </row>
     <row r="48" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="31"/>
-      <c r="C48" s="81"/>
-      <c r="D48" s="82"/>
+      <c r="C48" s="103"/>
+      <c r="D48" s="104"/>
       <c r="E48" s="2"/>
       <c r="F48" s="14"/>
       <c r="G48" s="2"/>
@@ -9572,58 +9572,58 @@
     </row>
     <row r="50" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11"/>
-      <c r="B50" s="110" t="s">
+      <c r="B50" s="128" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="111"/>
-      <c r="D50" s="111"/>
-      <c r="E50" s="111"/>
+      <c r="C50" s="129"/>
+      <c r="D50" s="129"/>
+      <c r="E50" s="129"/>
       <c r="F50" s="14"/>
-      <c r="G50" s="107" t="s">
+      <c r="G50" s="125" t="s">
         <v>83</v>
       </c>
-      <c r="H50" s="108"/>
-      <c r="I50" s="108"/>
-      <c r="J50" s="108"/>
-      <c r="K50" s="108"/>
-      <c r="L50" s="108"/>
-      <c r="M50" s="109"/>
+      <c r="H50" s="126"/>
+      <c r="I50" s="126"/>
+      <c r="J50" s="126"/>
+      <c r="K50" s="126"/>
+      <c r="L50" s="126"/>
+      <c r="M50" s="127"/>
     </row>
     <row r="51" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="112" t="s">
+      <c r="A51" s="130" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="113"/>
-      <c r="C51" s="113"/>
-      <c r="D51" s="113"/>
-      <c r="E51" s="113"/>
-      <c r="F51" s="114"/>
-      <c r="G51" s="83" t="s">
+      <c r="B51" s="131"/>
+      <c r="C51" s="131"/>
+      <c r="D51" s="131"/>
+      <c r="E51" s="131"/>
+      <c r="F51" s="132"/>
+      <c r="G51" s="105" t="s">
         <v>82</v>
       </c>
-      <c r="H51" s="84"/>
-      <c r="I51" s="84"/>
-      <c r="J51" s="84"/>
-      <c r="K51" s="84"/>
-      <c r="L51" s="84"/>
-      <c r="M51" s="85"/>
+      <c r="H51" s="106"/>
+      <c r="I51" s="106"/>
+      <c r="J51" s="106"/>
+      <c r="K51" s="106"/>
+      <c r="L51" s="106"/>
+      <c r="M51" s="107"/>
     </row>
     <row r="52" spans="1:13" s="16" customFormat="1" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
-      <c r="B52" s="103" t="s">
+      <c r="B52" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="103"/>
-      <c r="D52" s="103"/>
-      <c r="E52" s="103"/>
-      <c r="F52" s="103"/>
-      <c r="G52" s="103"/>
-      <c r="H52" s="103"/>
-      <c r="I52" s="103"/>
-      <c r="J52" s="103"/>
-      <c r="K52" s="103"/>
-      <c r="L52" s="103"/>
-      <c r="M52" s="104"/>
+      <c r="C52" s="94"/>
+      <c r="D52" s="94"/>
+      <c r="E52" s="94"/>
+      <c r="F52" s="94"/>
+      <c r="G52" s="94"/>
+      <c r="H52" s="94"/>
+      <c r="I52" s="94"/>
+      <c r="J52" s="94"/>
+      <c r="K52" s="94"/>
+      <c r="L52" s="94"/>
+      <c r="M52" s="95"/>
     </row>
     <row r="53" spans="1:13" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
@@ -9669,13 +9669,13 @@
       <c r="F55" s="14"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
-      <c r="I55" s="115" t="s">
+      <c r="I55" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="J55" s="115"/>
-      <c r="K55" s="115"/>
-      <c r="L55" s="115"/>
-      <c r="M55" s="116"/>
+      <c r="J55" s="82"/>
+      <c r="K55" s="82"/>
+      <c r="L55" s="82"/>
+      <c r="M55" s="83"/>
     </row>
     <row r="56" spans="1:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11"/>
@@ -9724,13 +9724,13 @@
       <c r="F58" s="14"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
-      <c r="I58" s="115" t="s">
+      <c r="I58" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="J58" s="115"/>
-      <c r="K58" s="115"/>
-      <c r="L58" s="115"/>
-      <c r="M58" s="116"/>
+      <c r="J58" s="82"/>
+      <c r="K58" s="82"/>
+      <c r="L58" s="82"/>
+      <c r="M58" s="83"/>
     </row>
     <row r="59" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11"/>
@@ -9743,13 +9743,13 @@
       <c r="F59" s="14"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
-      <c r="I59" s="115" t="s">
+      <c r="I59" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="J59" s="115"/>
-      <c r="K59" s="115"/>
-      <c r="L59" s="115"/>
-      <c r="M59" s="116"/>
+      <c r="J59" s="82"/>
+      <c r="K59" s="82"/>
+      <c r="L59" s="82"/>
+      <c r="M59" s="83"/>
     </row>
     <row r="60" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="11"/>
@@ -9762,44 +9762,44 @@
       <c r="F60" s="14"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
-      <c r="I60" s="115" t="s">
+      <c r="I60" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="J60" s="115"/>
-      <c r="K60" s="115"/>
-      <c r="L60" s="115"/>
-      <c r="M60" s="116"/>
+      <c r="J60" s="82"/>
+      <c r="K60" s="82"/>
+      <c r="L60" s="82"/>
+      <c r="M60" s="83"/>
     </row>
     <row r="61" spans="1:13" s="45" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="44"/>
-      <c r="G61" s="130" t="s">
+      <c r="G61" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="H61" s="131"/>
-      <c r="I61" s="131"/>
-      <c r="J61" s="131"/>
-      <c r="K61" s="131"/>
-      <c r="L61" s="131"/>
-      <c r="M61" s="132"/>
+      <c r="H61" s="78"/>
+      <c r="I61" s="78"/>
+      <c r="J61" s="78"/>
+      <c r="K61" s="78"/>
+      <c r="L61" s="78"/>
+      <c r="M61" s="79"/>
     </row>
     <row r="62" spans="1:13" s="49" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="47"/>
       <c r="B62" s="37"/>
-      <c r="C62" s="87" t="s">
+      <c r="C62" s="109" t="s">
         <v>62</v>
       </c>
-      <c r="D62" s="87"/>
-      <c r="E62" s="87"/>
+      <c r="D62" s="109"/>
+      <c r="E62" s="109"/>
       <c r="F62" s="48"/>
-      <c r="G62" s="88" t="s">
+      <c r="G62" s="110" t="s">
         <v>73</v>
       </c>
-      <c r="H62" s="89"/>
-      <c r="I62" s="84"/>
-      <c r="J62" s="84"/>
-      <c r="K62" s="84"/>
-      <c r="L62" s="84"/>
-      <c r="M62" s="90"/>
+      <c r="H62" s="111"/>
+      <c r="I62" s="106"/>
+      <c r="J62" s="106"/>
+      <c r="K62" s="106"/>
+      <c r="L62" s="106"/>
+      <c r="M62" s="112"/>
     </row>
     <row r="63" spans="1:13" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
@@ -9829,14 +9829,14 @@
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="133" t="s">
+      <c r="H64" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="I64" s="133"/>
-      <c r="J64" s="133"/>
-      <c r="K64" s="133"/>
-      <c r="L64" s="133"/>
-      <c r="M64" s="134"/>
+      <c r="I64" s="80"/>
+      <c r="J64" s="80"/>
+      <c r="K64" s="80"/>
+      <c r="L64" s="80"/>
+      <c r="M64" s="81"/>
     </row>
     <row r="65" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="11"/>
@@ -9847,14 +9847,14 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="H65" s="115" t="s">
+      <c r="H65" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="I65" s="115"/>
-      <c r="J65" s="115"/>
-      <c r="K65" s="115"/>
-      <c r="L65" s="115"/>
-      <c r="M65" s="116"/>
+      <c r="I65" s="82"/>
+      <c r="J65" s="82"/>
+      <c r="K65" s="82"/>
+      <c r="L65" s="82"/>
+      <c r="M65" s="83"/>
     </row>
     <row r="66" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="11"/>
@@ -9865,14 +9865,14 @@
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-      <c r="H66" s="115" t="s">
+      <c r="H66" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="I66" s="115"/>
-      <c r="J66" s="115"/>
-      <c r="K66" s="115"/>
-      <c r="L66" s="115"/>
-      <c r="M66" s="116"/>
+      <c r="I66" s="82"/>
+      <c r="J66" s="82"/>
+      <c r="K66" s="82"/>
+      <c r="L66" s="82"/>
+      <c r="M66" s="83"/>
     </row>
     <row r="67" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="11"/>
@@ -9889,102 +9889,112 @@
       <c r="M67" s="14"/>
     </row>
     <row r="68" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="91" t="s">
+      <c r="A68" s="113" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="92"/>
-      <c r="C68" s="92"/>
-      <c r="D68" s="92"/>
-      <c r="E68" s="92"/>
-      <c r="F68" s="92"/>
-      <c r="G68" s="92"/>
-      <c r="H68" s="92"/>
-      <c r="I68" s="92"/>
-      <c r="J68" s="92"/>
-      <c r="K68" s="92"/>
-      <c r="L68" s="92"/>
-      <c r="M68" s="93"/>
+      <c r="B68" s="114"/>
+      <c r="C68" s="114"/>
+      <c r="D68" s="114"/>
+      <c r="E68" s="114"/>
+      <c r="F68" s="114"/>
+      <c r="G68" s="114"/>
+      <c r="H68" s="114"/>
+      <c r="I68" s="114"/>
+      <c r="J68" s="114"/>
+      <c r="K68" s="114"/>
+      <c r="L68" s="114"/>
+      <c r="M68" s="115"/>
     </row>
     <row r="69" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="94" t="s">
+      <c r="A69" s="116" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="95"/>
-      <c r="C69" s="95"/>
-      <c r="D69" s="95"/>
-      <c r="E69" s="95"/>
-      <c r="F69" s="95"/>
-      <c r="G69" s="95"/>
-      <c r="H69" s="95"/>
-      <c r="I69" s="95"/>
-      <c r="J69" s="95"/>
-      <c r="K69" s="95"/>
-      <c r="L69" s="95"/>
-      <c r="M69" s="96"/>
+      <c r="B69" s="117"/>
+      <c r="C69" s="117"/>
+      <c r="D69" s="117"/>
+      <c r="E69" s="117"/>
+      <c r="F69" s="117"/>
+      <c r="G69" s="117"/>
+      <c r="H69" s="117"/>
+      <c r="I69" s="117"/>
+      <c r="J69" s="117"/>
+      <c r="K69" s="117"/>
+      <c r="L69" s="117"/>
+      <c r="M69" s="118"/>
     </row>
     <row r="70" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="97" t="s">
+      <c r="A70" s="119" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="98"/>
-      <c r="C70" s="98"/>
-      <c r="D70" s="98"/>
-      <c r="E70" s="98"/>
-      <c r="F70" s="98"/>
-      <c r="G70" s="98"/>
-      <c r="H70" s="98"/>
-      <c r="I70" s="98"/>
-      <c r="J70" s="98"/>
-      <c r="K70" s="98"/>
-      <c r="L70" s="98"/>
-      <c r="M70" s="99"/>
+      <c r="B70" s="120"/>
+      <c r="C70" s="120"/>
+      <c r="D70" s="120"/>
+      <c r="E70" s="120"/>
+      <c r="F70" s="120"/>
+      <c r="G70" s="120"/>
+      <c r="H70" s="120"/>
+      <c r="I70" s="120"/>
+      <c r="J70" s="120"/>
+      <c r="K70" s="120"/>
+      <c r="L70" s="120"/>
+      <c r="M70" s="121"/>
     </row>
     <row r="71" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="100" t="s">
+      <c r="A71" s="122" t="s">
         <v>72</v>
       </c>
-      <c r="B71" s="101"/>
-      <c r="C71" s="101"/>
-      <c r="D71" s="101"/>
-      <c r="E71" s="101"/>
-      <c r="F71" s="101"/>
-      <c r="G71" s="101"/>
-      <c r="H71" s="101"/>
-      <c r="I71" s="101"/>
-      <c r="J71" s="101"/>
-      <c r="K71" s="101"/>
-      <c r="L71" s="101"/>
-      <c r="M71" s="102"/>
+      <c r="B71" s="123"/>
+      <c r="C71" s="123"/>
+      <c r="D71" s="123"/>
+      <c r="E71" s="123"/>
+      <c r="F71" s="123"/>
+      <c r="G71" s="123"/>
+      <c r="H71" s="123"/>
+      <c r="I71" s="123"/>
+      <c r="J71" s="123"/>
+      <c r="K71" s="123"/>
+      <c r="L71" s="123"/>
+      <c r="M71" s="124"/>
     </row>
     <row r="72" spans="1:13" s="52" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="86"/>
-      <c r="B72" s="86"/>
-      <c r="C72" s="86"/>
-      <c r="D72" s="86"/>
-      <c r="E72" s="86"/>
-      <c r="F72" s="86"/>
-      <c r="G72" s="86"/>
-      <c r="H72" s="86"/>
-      <c r="I72" s="86"/>
-      <c r="J72" s="86"/>
-      <c r="K72" s="86"/>
-      <c r="L72" s="86"/>
-      <c r="M72" s="86"/>
+      <c r="A72" s="108"/>
+      <c r="B72" s="108"/>
+      <c r="C72" s="108"/>
+      <c r="D72" s="108"/>
+      <c r="E72" s="108"/>
+      <c r="F72" s="108"/>
+      <c r="G72" s="108"/>
+      <c r="H72" s="108"/>
+      <c r="I72" s="108"/>
+      <c r="J72" s="108"/>
+      <c r="K72" s="108"/>
+      <c r="L72" s="108"/>
+      <c r="M72" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="G61:M61"/>
-    <mergeCell ref="H64:M64"/>
-    <mergeCell ref="H65:M65"/>
-    <mergeCell ref="H66:M66"/>
-    <mergeCell ref="I58:M58"/>
-    <mergeCell ref="I59:M59"/>
-    <mergeCell ref="I60:M60"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="O43:P43"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="G51:M51"/>
+    <mergeCell ref="A72:M72"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="G62:M62"/>
+    <mergeCell ref="A68:M68"/>
+    <mergeCell ref="A69:M69"/>
+    <mergeCell ref="A70:M70"/>
+    <mergeCell ref="A71:M71"/>
+    <mergeCell ref="B52:M52"/>
+    <mergeCell ref="I47:M47"/>
+    <mergeCell ref="G50:M50"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="I55:M55"/>
     <mergeCell ref="H37:M37"/>
     <mergeCell ref="I41:M41"/>
     <mergeCell ref="I39:M39"/>
@@ -10001,28 +10011,18 @@
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="H11:M11"/>
     <mergeCell ref="H17:M17"/>
-    <mergeCell ref="O43:P43"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="G51:M51"/>
-    <mergeCell ref="A72:M72"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="G62:M62"/>
-    <mergeCell ref="A68:M68"/>
-    <mergeCell ref="A69:M69"/>
-    <mergeCell ref="A70:M70"/>
-    <mergeCell ref="A71:M71"/>
-    <mergeCell ref="B52:M52"/>
-    <mergeCell ref="I47:M47"/>
-    <mergeCell ref="G50:M50"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="I55:M55"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="G61:M61"/>
+    <mergeCell ref="H64:M64"/>
+    <mergeCell ref="H65:M65"/>
+    <mergeCell ref="H66:M66"/>
+    <mergeCell ref="I58:M58"/>
+    <mergeCell ref="I59:M59"/>
+    <mergeCell ref="I60:M60"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="K27:M27"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10609,42 +10609,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="133" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="74"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
+      <c r="A2" s="134"/>
+      <c r="B2" s="134"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="135" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
+      <c r="B3" s="135"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="135"/>
+      <c r="G3" s="135"/>
+      <c r="H3" s="135"/>
+      <c r="I3" s="135"/>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -10666,14 +10666,14 @@
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="135"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="136"/>
+      <c r="B5" s="140"/>
+      <c r="C5" s="137"/>
+      <c r="D5" s="137"/>
+      <c r="E5" s="137"/>
+      <c r="F5" s="137"/>
+      <c r="G5" s="137"/>
+      <c r="H5" s="137"/>
+      <c r="I5" s="141"/>
     </row>
     <row r="6" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
@@ -10702,16 +10702,16 @@
     </row>
     <row r="8" spans="1:11" s="16" customFormat="1" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="103"/>
-      <c r="F8" s="103"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="104"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="95"/>
     </row>
     <row r="9" spans="1:11" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
@@ -11004,12 +11004,12 @@
     <row r="31" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="125" t="s">
+      <c r="C31" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="125"/>
-      <c r="E31" s="125"/>
-      <c r="F31" s="126"/>
+      <c r="D31" s="96"/>
+      <c r="E31" s="96"/>
+      <c r="F31" s="97"/>
       <c r="G31" s="2"/>
       <c r="H31" s="23" t="s">
         <v>30</v>
@@ -11170,8 +11170,8 @@
         <v>41</v>
       </c>
       <c r="I43" s="26"/>
-      <c r="K43" s="79"/>
-      <c r="L43" s="80"/>
+      <c r="K43" s="101"/>
+      <c r="L43" s="102"/>
     </row>
     <row r="44" spans="1:12" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="29"/>
@@ -11227,8 +11227,8 @@
     <row r="48" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
       <c r="B48" s="31"/>
-      <c r="C48" s="79"/>
-      <c r="D48" s="80"/>
+      <c r="C48" s="101"/>
+      <c r="D48" s="102"/>
       <c r="E48" s="2"/>
       <c r="F48" s="14"/>
       <c r="G48" s="2"/>
@@ -11266,30 +11266,30 @@
         <v>47</v>
       </c>
       <c r="B51" s="2"/>
-      <c r="C51" s="89" t="s">
+      <c r="C51" s="111" t="s">
         <v>73</v>
       </c>
-      <c r="D51" s="84"/>
+      <c r="D51" s="106"/>
       <c r="E51" s="37"/>
       <c r="F51" s="14"/>
-      <c r="G51" s="137" t="s">
+      <c r="G51" s="139" t="s">
         <v>48</v>
       </c>
-      <c r="H51" s="84"/>
-      <c r="I51" s="85"/>
+      <c r="H51" s="106"/>
+      <c r="I51" s="107"/>
     </row>
     <row r="52" spans="1:9" s="16" customFormat="1" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
-      <c r="B52" s="103" t="s">
+      <c r="B52" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="103"/>
-      <c r="D52" s="103"/>
-      <c r="E52" s="103"/>
-      <c r="F52" s="103"/>
-      <c r="G52" s="103"/>
-      <c r="H52" s="103"/>
-      <c r="I52" s="104"/>
+      <c r="C52" s="94"/>
+      <c r="D52" s="94"/>
+      <c r="E52" s="94"/>
+      <c r="F52" s="94"/>
+      <c r="G52" s="94"/>
+      <c r="H52" s="94"/>
+      <c r="I52" s="95"/>
     </row>
     <row r="53" spans="1:9" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
@@ -11414,17 +11414,17 @@
     <row r="62" spans="1:9" s="49" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="47"/>
       <c r="B62" s="37"/>
-      <c r="C62" s="87" t="s">
+      <c r="C62" s="109" t="s">
         <v>62</v>
       </c>
-      <c r="D62" s="87"/>
-      <c r="E62" s="87"/>
+      <c r="D62" s="109"/>
+      <c r="E62" s="109"/>
       <c r="F62" s="48"/>
-      <c r="G62" s="88" t="s">
+      <c r="G62" s="110" t="s">
         <v>73</v>
       </c>
-      <c r="H62" s="84"/>
-      <c r="I62" s="90"/>
+      <c r="H62" s="106"/>
+      <c r="I62" s="112"/>
     </row>
     <row r="63" spans="1:9" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
@@ -11494,70 +11494,77 @@
       <c r="I67" s="14"/>
     </row>
     <row r="68" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="91" t="s">
+      <c r="A68" s="113" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="92"/>
-      <c r="C68" s="92"/>
-      <c r="D68" s="92"/>
-      <c r="E68" s="92"/>
-      <c r="F68" s="92"/>
-      <c r="G68" s="92"/>
-      <c r="H68" s="92"/>
-      <c r="I68" s="93"/>
+      <c r="B68" s="114"/>
+      <c r="C68" s="114"/>
+      <c r="D68" s="114"/>
+      <c r="E68" s="114"/>
+      <c r="F68" s="114"/>
+      <c r="G68" s="114"/>
+      <c r="H68" s="114"/>
+      <c r="I68" s="115"/>
     </row>
     <row r="69" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="94" t="s">
+      <c r="A69" s="116" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="95"/>
-      <c r="C69" s="95"/>
-      <c r="D69" s="95"/>
-      <c r="E69" s="95"/>
-      <c r="F69" s="95"/>
-      <c r="G69" s="95"/>
-      <c r="H69" s="95"/>
-      <c r="I69" s="96"/>
+      <c r="B69" s="117"/>
+      <c r="C69" s="117"/>
+      <c r="D69" s="117"/>
+      <c r="E69" s="117"/>
+      <c r="F69" s="117"/>
+      <c r="G69" s="117"/>
+      <c r="H69" s="117"/>
+      <c r="I69" s="118"/>
     </row>
     <row r="70" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="97" t="s">
+      <c r="A70" s="119" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="98"/>
-      <c r="C70" s="98"/>
-      <c r="D70" s="98"/>
-      <c r="E70" s="98"/>
-      <c r="F70" s="98"/>
-      <c r="G70" s="98"/>
-      <c r="H70" s="98"/>
-      <c r="I70" s="99"/>
+      <c r="B70" s="120"/>
+      <c r="C70" s="120"/>
+      <c r="D70" s="120"/>
+      <c r="E70" s="120"/>
+      <c r="F70" s="120"/>
+      <c r="G70" s="120"/>
+      <c r="H70" s="120"/>
+      <c r="I70" s="121"/>
     </row>
     <row r="71" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="100" t="s">
+      <c r="A71" s="122" t="s">
         <v>72</v>
       </c>
-      <c r="B71" s="101"/>
-      <c r="C71" s="101"/>
-      <c r="D71" s="101"/>
-      <c r="E71" s="101"/>
-      <c r="F71" s="101"/>
-      <c r="G71" s="101"/>
-      <c r="H71" s="101"/>
-      <c r="I71" s="102"/>
+      <c r="B71" s="123"/>
+      <c r="C71" s="123"/>
+      <c r="D71" s="123"/>
+      <c r="E71" s="123"/>
+      <c r="F71" s="123"/>
+      <c r="G71" s="123"/>
+      <c r="H71" s="123"/>
+      <c r="I71" s="124"/>
     </row>
     <row r="72" spans="1:9" s="52" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="86"/>
-      <c r="B72" s="86"/>
-      <c r="C72" s="86"/>
-      <c r="D72" s="86"/>
-      <c r="E72" s="86"/>
-      <c r="F72" s="86"/>
-      <c r="G72" s="86"/>
-      <c r="H72" s="86"/>
-      <c r="I72" s="86"/>
+      <c r="A72" s="108"/>
+      <c r="B72" s="108"/>
+      <c r="C72" s="108"/>
+      <c r="D72" s="108"/>
+      <c r="E72" s="108"/>
+      <c r="F72" s="108"/>
+      <c r="G72" s="108"/>
+      <c r="H72" s="108"/>
+      <c r="I72" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:I5"/>
     <mergeCell ref="K43:L43"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="C51:D51"/>
@@ -11570,13 +11577,6 @@
     <mergeCell ref="A70:I70"/>
     <mergeCell ref="A71:I71"/>
     <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:I5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>